<commit_message>
Add reports controlle to show reports and use before_save callback
</commit_message>
<xml_diff>
--- a/public/report.xlsx
+++ b/public/report.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="36" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="37" xml:space="preserve">
   <si>
     <t>Quiz name</t>
   </si>
@@ -117,6 +117,9 @@
   </si>
   <si>
     <t>sanjibrnjnjndjndjndoy0098@gmail.com</t>
+  </si>
+  <si>
+    <t>sanjibrosnjssjnjy0098@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -180,7 +183,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -703,6 +706,23 @@
         <v>1</v>
       </c>
     </row>
+    <row r="31">
+      <c r="A31" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E31" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <printOptions verticalCentered="0" horizontalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Built reusable QuestionForm component and remove redundant code from add and edit question
</commit_message>
<xml_diff>
--- a/public/report.xlsx
+++ b/public/report.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="37" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="40" xml:space="preserve">
   <si>
     <t>Quiz name</t>
   </si>
@@ -120,6 +120,15 @@
   </si>
   <si>
     <t>sanjibrosnjssjnjy0098@gmail.com</t>
+  </si>
+  <si>
+    <t>sanjibroy53110098@gmail.com</t>
+  </si>
+  <si>
+    <t>sanjibroy00444698@gmail.com</t>
+  </si>
+  <si>
+    <t>san4646546jibroy0098@gmail.com</t>
   </si>
 </sst>
 </file>
@@ -183,7 +192,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E31"/>
+  <dimension ref="A1:E35"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -326,10 +335,10 @@
         <v>13</v>
       </c>
       <c r="D8" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E8" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9">
@@ -377,10 +386,10 @@
         <v>16</v>
       </c>
       <c r="D11" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E11" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="12">
@@ -411,10 +420,10 @@
         <v>18</v>
       </c>
       <c r="D13" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E13" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
     </row>
     <row r="14">
@@ -428,10 +437,10 @@
         <v>19</v>
       </c>
       <c r="D14" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E14" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="15">
@@ -445,10 +454,10 @@
         <v>20</v>
       </c>
       <c r="D15" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E15" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="16">
@@ -462,10 +471,10 @@
         <v>21</v>
       </c>
       <c r="D16" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E16" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="17">
@@ -547,10 +556,10 @@
         <v>26</v>
       </c>
       <c r="D21" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E21" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="22">
@@ -649,10 +658,10 @@
         <v>32</v>
       </c>
       <c r="D27" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E27" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="28">
@@ -700,10 +709,10 @@
         <v>35</v>
       </c>
       <c r="D30" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E30" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="31">
@@ -717,10 +726,78 @@
         <v>36</v>
       </c>
       <c r="D31" s="0" t="n">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="E31" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>25</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E32" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E33" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E34" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E35" s="0" t="n">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Follow RESTful convention and refactor code
</commit_message>
<xml_diff>
--- a/public/report.xlsx
+++ b/public/report.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="11" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12" xml:space="preserve">
   <si>
     <t>Quiz name</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>sanjibroysnjsnsj0098@gmail.com</t>
+  </si>
+  <si>
+    <t>Bengali</t>
   </si>
 </sst>
 </file>
@@ -105,7 +108,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -203,6 +206,23 @@
         <v>0</v>
       </c>
     </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <sheetCalcPr fullCalcOnLoad="1"/>
   <printOptions verticalCentered="0" horizontalCentered="0" headings="0" gridLines="0"/>

</xml_diff>

<commit_message>
Redirect to the home page if quiz slug is invalid.
</commit_message>
<xml_diff>
--- a/public/report.xlsx
+++ b/public/report.xlsx
@@ -9,7 +9,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12" xml:space="preserve">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="15" xml:space="preserve">
   <si>
     <t>Quiz name</t>
   </si>
@@ -35,16 +35,25 @@
     <t>sanjibroy0098@gmail.com</t>
   </si>
   <si>
-    <t>sanjibroyndjndjdj0098@gmail.com</t>
-  </si>
-  <si>
-    <t>sanjinjnjnjsbroy0098@gmail.com</t>
-  </si>
-  <si>
-    <t>sanjibroysnjsnsj0098@gmail.com</t>
-  </si>
-  <si>
-    <t>Bengali</t>
+    <t>sanjibroy0099@gmail.com</t>
+  </si>
+  <si>
+    <t>sanjibroy01@gmail.com</t>
+  </si>
+  <si>
+    <t>sanjibroy@gmail.com</t>
+  </si>
+  <si>
+    <t>sanjibroy0095@gmail.com</t>
+  </si>
+  <si>
+    <t>sanjibronjjknkj@gmail.com</t>
+  </si>
+  <si>
+    <t>sanjibroybjhbjhbhjbhj0098@gmail.com</t>
+  </si>
+  <si>
+    <t>Test Quiz</t>
   </si>
 </sst>
 </file>
@@ -108,7 +117,7 @@
   <sheetPr>
     <pageSetUpPr fitToPage="0"/>
   </sheetPr>
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView windowProtection="0" tabSelected="0" showWhiteSpace="0" showOutlineSymbols="0" showFormulas="0" rightToLeft="0" showZeros="1" showRuler="1" showRowColHeaders="1" showGridLines="1" defaultGridColor="1" zoomScale="100" workbookViewId="0" zoomScaleSheetLayoutView="0" zoomScalePageLayoutView="0" zoomScaleNormal="0"/>
   </sheetViews>
@@ -116,7 +125,7 @@
   <cols>
     <col min="1" max="1" bestFit="1" customWidth="1" width="13.200000000000001"/>
     <col min="2" max="2" bestFit="1" customWidth="1" width="14.3"/>
-    <col min="3" max="3" bestFit="1" customWidth="1" width="37.400000000000006"/>
+    <col min="3" max="3" bestFit="1" customWidth="1" width="41.800000000000004"/>
     <col min="4" max="4" bestFit="1" customWidth="1" width="19.8"/>
     <col min="5" max="5" bestFit="1" customWidth="1" width="22.0"/>
   </cols>
@@ -152,7 +161,7 @@
         <v>0</v>
       </c>
       <c r="E2" s="0" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="3">
@@ -166,10 +175,10 @@
         <v>8</v>
       </c>
       <c r="D3" s="0" t="n">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="E3" s="0" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4">
@@ -183,7 +192,7 @@
         <v>9</v>
       </c>
       <c r="D4" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E4" s="0" t="n">
         <v>1</v>
@@ -200,26 +209,77 @@
         <v>10</v>
       </c>
       <c r="D5" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E5" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="0" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="0" t="s">
+      <c r="D6" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E6" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="E7" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="E8" s="0" t="n">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="E6" s="0" t="n">
+      <c r="D9" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="E9" s="0" t="n">
         <v>1</v>
       </c>
     </row>

</xml_diff>